<commit_message>
Added Logger functionality with parallel run
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/TestCases.xlsx
+++ b/src/test/resources/ExcelFiles/TestCases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="67">
   <si>
     <t>Scenario Steps</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>chrome</t>
@@ -567,7 +564,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +575,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>51</v>
@@ -589,7 +586,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
@@ -600,35 +597,35 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +681,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Extent report with thread safe and error screenshot
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/TestCases.xlsx
+++ b/src/test/resources/ExcelFiles/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="70">
   <si>
     <t>Scenario Steps</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t>With opera browser</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>//label[text()='First Name']</t>
   </si>
 </sst>
 </file>
@@ -563,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +612,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +623,7 @@
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,7 +634,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +647,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +894,7 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1166,7 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -1194,7 +1203,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>